<commit_message>
SP1 Sprint Planning e Casos de uso v1.0
</commit_message>
<xml_diff>
--- a/PréGame/Regra para distribuição de papeis.xlsx
+++ b/PréGame/Regra para distribuição de papeis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -207,16 +207,6 @@
         <family val="2"/>
       </rPr>
       <t>Analista de qualidade (8)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t>relatório de testes</t>
     </r>
   </si>
   <si>
@@ -299,11 +289,38 @@
   <si>
     <t>Matheus e Nicholas</t>
   </si>
+  <si>
+    <t xml:space="preserve">O QUE FAZER? </t>
+  </si>
+  <si>
+    <t>Cronograma v2.0 , EAP v2.0</t>
+  </si>
+  <si>
+    <t>Plano de testes</t>
+  </si>
+  <si>
+    <t>Planilha de riscos</t>
+  </si>
+  <si>
+    <t>Modelo do BD</t>
+  </si>
+  <si>
+    <t>Diagramas</t>
+  </si>
+  <si>
+    <t>Casos de uso</t>
+  </si>
+  <si>
+    <t>Código fonte v1.0</t>
+  </si>
+  <si>
+    <t>relatório de testes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0;###0"/>
   </numFmts>
@@ -548,6 +565,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -582,6 +600,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -757,11 +776,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -771,6 +790,7 @@
     <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="6" max="6" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -781,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -789,7 +809,9 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -799,11 +821,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -813,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -827,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -841,13 +865,15 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -857,7 +883,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="5">
@@ -873,71 +899,81 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.1" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
+      <c r="B9" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="10"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
Sprint Planning - Sprint 2
</commit_message>
<xml_diff>
--- a/PréGame/Regra para distribuição de papeis.xlsx
+++ b/PréGame/Regra para distribuição de papeis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
@@ -166,16 +166,6 @@
         <rFont val="DejaVu Sans"/>
         <family val="2"/>
       </rPr>
-      <t>Casos de testes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
       <t>Analista de BD (6)</t>
     </r>
   </si>
@@ -316,11 +306,14 @@
   <si>
     <t>relatório de testes</t>
   </si>
+  <si>
+    <t>Casos de testes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0;###0"/>
   </numFmts>
@@ -565,7 +558,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -600,7 +592,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -776,11 +767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -801,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -810,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
@@ -821,12 +812,12 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
@@ -837,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -851,7 +842,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -865,25 +856,25 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
+      <c r="B6" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="5">
@@ -893,78 +884,78 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.1" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11" t="s">
@@ -972,7 +963,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6">

</xml_diff>